<commit_message>
gitignore and readme file modified
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\django\product_importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4BAD9CB-7007-4E73-B962-5701E2606815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A53F2E6-8A28-4EE8-94CF-1FD650130388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{744271D3-C708-40E1-9CC8-7B2CFF84DC0A}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +430,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>